<commit_message>
Add display_url field to image/ad_tag creatives. (#3597)
</commit_message>
<xml_diff>
--- a/client/one/assets/Zemanta_Display_Ads_Template.xlsx
+++ b/client/one/assets/Zemanta_Display_Ads_Template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>URL</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Ad tag</t>
+  </si>
+  <si>
+    <t>Display URL</t>
   </si>
   <si>
     <t>Label</t>
@@ -46,6 +49,25 @@
     <t>300x250</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>www.</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>zemanta.com</t>
+    </r>
+  </si>
+  <si>
     <t>Blog Content</t>
   </si>
   <si>
@@ -59,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -73,6 +95,12 @@
     <font>
       <sz val="15"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -151,6 +179,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1212,14 +1241,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="10.8516" style="1" customWidth="1"/>
-    <col min="9" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="5" width="10.8516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.8516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.8516" style="1" customWidth="1"/>
+    <col min="10" max="256" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
@@ -1247,27 +1280,33 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" ht="17" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I2" t="s" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="17" customHeight="1">
@@ -1279,6 +1318,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" s="3"/>
@@ -1289,6 +1329,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" s="3"/>
@@ -1299,6 +1340,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" s="3"/>
@@ -1309,6 +1351,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" ht="17" customHeight="1">
       <c r="A7" s="3"/>
@@ -1319,6 +1362,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="3"/>
@@ -1329,6 +1373,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" s="3"/>
@@ -1339,6 +1384,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" s="3"/>
@@ -1349,8 +1395,12 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>